<commit_message>
final for 2E python section
</commit_message>
<xml_diff>
--- a/02-output/wine_country_stats/Q2E_Argentina.xlsx
+++ b/02-output/wine_country_stats/Q2E_Argentina.xlsx
@@ -14,18 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Statistic</t>
   </si>
   <si>
-    <t>Argentina price price</t>
-  </si>
-  <si>
-    <t>_1</t>
-  </si>
-  <si>
-    <t>Argentina points points</t>
+    <t>Argentina_priceprice</t>
+  </si>
+  <si>
+    <t>Argentina_pointspoints</t>
   </si>
   <si>
     <t>Count</t>
@@ -407,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -419,12 +416,11 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -434,95 +430,92 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
       </c>
       <c r="B2">
         <v>3714</v>
       </c>
-      <c r="D2">
+      <c r="C2">
         <v>3714</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>24.57915993537964</v>
       </c>
-      <c r="D3">
+      <c r="C3">
         <v>86.73451803984922</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>23.54408753591872</v>
       </c>
-      <c r="D4">
+      <c r="C4">
         <v>3.180122531050384</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="D5">
+      <c r="C5">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>12</v>
       </c>
-      <c r="D6">
+      <c r="C6">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>17</v>
       </c>
-      <c r="D7">
+      <c r="C7">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>25</v>
       </c>
-      <c r="D8">
+      <c r="C8">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>230</v>
       </c>
-      <c r="D9">
+      <c r="C9">
         <v>97</v>
       </c>
     </row>

</xml_diff>